<commit_message>
refactored Flip() to call CheckWinner()
</commit_message>
<xml_diff>
--- a/assets/schema.xlsx
+++ b/assets/schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gyzub\codefellows\401\speed-war\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A694812E-335E-452C-B9C0-CC38986815C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D86417-77EB-4C9F-A1D2-F944A64FA21D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="16875" windowHeight="10522" xr2:uid="{CB711FC9-8CB4-45EE-A040-2F7F8A0B484A}"/>
+    <workbookView xWindow="653" yWindow="2940" windowWidth="19162" windowHeight="10522" xr2:uid="{CB711FC9-8CB4-45EE-A040-2F7F8A0B484A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>NAV PROPS</t>
   </si>
@@ -57,18 +57,6 @@
     <t>Rank</t>
   </si>
   <si>
-    <t>Ace</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Queen</t>
-  </si>
-  <si>
-    <t>King</t>
-  </si>
-  <si>
     <t>CardID</t>
   </si>
   <si>
@@ -136,6 +124,45 @@
   </si>
   <si>
     <t>USER</t>
+  </si>
+  <si>
+    <t>Ace = 1</t>
+  </si>
+  <si>
+    <t>Two = 2</t>
+  </si>
+  <si>
+    <t>Three = 3</t>
+  </si>
+  <si>
+    <t>Four = 4</t>
+  </si>
+  <si>
+    <t>Five = 5</t>
+  </si>
+  <si>
+    <t>Six = 6</t>
+  </si>
+  <si>
+    <t>Seven = 7</t>
+  </si>
+  <si>
+    <t>Eight = 8</t>
+  </si>
+  <si>
+    <t>Nine = 9</t>
+  </si>
+  <si>
+    <t>Ten = 10</t>
+  </si>
+  <si>
+    <t>Jack = 11</t>
+  </si>
+  <si>
+    <t>Queen = 12</t>
+  </si>
+  <si>
+    <t>King = 13</t>
   </si>
 </sst>
 </file>
@@ -648,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804527C0-50A5-4157-ACA9-2204E729FD9A}">
   <dimension ref="B1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13:R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -677,27 +704,27 @@
     <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="12"/>
       <c r="J2" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="12"/>
       <c r="N2" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="12"/>
       <c r="R2" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.45">
@@ -711,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>3</v>
@@ -738,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.45">
@@ -750,22 +777,22 @@
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" t="s">
@@ -775,7 +802,7 @@
         <v>3</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -790,15 +817,15 @@
       <c r="H5" s="4"/>
       <c r="J5" s="3"/>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N5" s="3"/>
       <c r="P5" s="4"/>
       <c r="R5" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -817,7 +844,7 @@
       <c r="O6" s="11"/>
       <c r="P6" s="12"/>
       <c r="R6" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -828,7 +855,7 @@
       <c r="D7" s="12"/>
       <c r="F7" s="3"/>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H7" s="4"/>
       <c r="J7" s="10" t="s">
@@ -850,19 +877,19 @@
       <c r="D8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H8" s="4"/>
       <c r="J8" s="3"/>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L8" s="4"/>
       <c r="N8" s="5"/>
       <c r="O8" s="2"/>
       <c r="P8" s="6"/>
       <c r="R8" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -876,88 +903,88 @@
       <c r="K9" s="2"/>
       <c r="L9" s="6"/>
       <c r="R9" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.45">
       <c r="R10" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="R11" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="13" spans="2:18" x14ac:dyDescent="0.45">
       <c r="R13" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.45">
       <c r="R14" s="8" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="R15" s="8">
-        <v>2</v>
+      <c r="R15" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="R16" s="8">
-        <v>3</v>
+      <c r="R16" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="18:18" x14ac:dyDescent="0.45">
-      <c r="R17" s="8">
-        <v>4</v>
+      <c r="R17" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="18:18" x14ac:dyDescent="0.45">
-      <c r="R18" s="8">
-        <v>5</v>
+      <c r="R18" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="18:18" x14ac:dyDescent="0.45">
-      <c r="R19" s="8">
-        <v>6</v>
+      <c r="R19" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="18:18" x14ac:dyDescent="0.45">
-      <c r="R20" s="8">
-        <v>7</v>
+      <c r="R20" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="18:18" x14ac:dyDescent="0.45">
-      <c r="R21" s="8">
-        <v>8</v>
+      <c r="R21" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="18:18" x14ac:dyDescent="0.45">
-      <c r="R22" s="8">
-        <v>9</v>
+      <c r="R22" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="18:18" x14ac:dyDescent="0.45">
-      <c r="R23" s="8">
-        <v>10</v>
+      <c r="R23" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="18:18" x14ac:dyDescent="0.45">
       <c r="R24" s="8" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="18:18" x14ac:dyDescent="0.45">
       <c r="R25" s="8" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="18:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="R26" s="9" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>